<commit_message>
Updated Excel Datei für Unternehmen
Eigene Spalten für die jeden Zeitslot hinzugefügt.
</commit_message>
<xml_diff>
--- a/Unterrichtsmaterial/BetriebeExcel.xlsx
+++ b/Unterrichtsmaterial/BetriebeExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0498C512-8616-4360-A44D-7341E7970878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F9B0F51-CEA4-44E0-A6B5-0701AC2BB4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="38">
   <si>
     <t>Unternehmen</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Nr.</t>
   </si>
   <si>
-    <t>Zeitslots</t>
-  </si>
-  <si>
     <t>Gruppengroeße</t>
   </si>
   <si>
@@ -114,19 +111,34 @@
     <t>Sparkasse Aachen</t>
   </si>
   <si>
-    <t>A,B,C,D,E</t>
-  </si>
-  <si>
-    <t>C,D,E</t>
-  </si>
-  <si>
-    <t>A,B,C</t>
-  </si>
-  <si>
-    <t>B,C,D,E</t>
-  </si>
-  <si>
-    <t>A,B,C,D</t>
+    <t>Zeitslot A</t>
+  </si>
+  <si>
+    <t>Zeitslot B</t>
+  </si>
+  <si>
+    <t>Zeitslot C</t>
+  </si>
+  <si>
+    <t>Zeitslot D</t>
+  </si>
+  <si>
+    <t>Zeitslot E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -444,21 +456,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -466,388 +481,703 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
       <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>